<commit_message>
Ini Chat della loddy, invio e ricezione messaggi client/host
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Library\Communication\Messages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7F541-9808-4590-BFFB-BA3D3A711AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21F0F67-ED3F-49AC-8D12-144C58C92F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nome Messaggio</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Invia la lista aggiornata di utenti quanto se ne connette uno nuovo o si disconnette un nuovo utente</t>
+  </si>
+  <si>
+    <t>LobbyChatMessage</t>
+  </si>
+  <si>
+    <t>Contiene un messaggio testuale per della chat della lobby, e le informazioni del mittente</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,8 +512,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
       <c r="B6">
         <v>1004</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Gestito stato della chat (abilitato/disabilitato)
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21F0F67-ED3F-49AC-8D12-144C58C92F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4363C85-153F-4DE0-A756-215B28754932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Nome Messaggio</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Contiene un messaggio testuale per della chat della lobby, e le informazioni del mittente</t>
+  </si>
+  <si>
+    <t>ChangeLobbyChatStatus</t>
+  </si>
+  <si>
+    <t>Manda il nuovo stato (abilitata/disabilitata) della chat</t>
   </si>
 </sst>
 </file>
@@ -417,7 +423,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,6 +528,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>1005</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
     </row>

</xml_diff>

<commit_message>
Aggiunte classi base per Online Settings e per Online Game ViewModel
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4363C85-153F-4DE0-A756-215B28754932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220B0B0C-71A4-46C8-9779-DFB99D2073B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,10 +81,10 @@
     <t>Contiene un messaggio testuale per della chat della lobby, e le informazioni del mittente</t>
   </si>
   <si>
-    <t>ChangeLobbyChatStatus</t>
-  </si>
-  <si>
-    <t>Manda il nuovo stato (abilitata/disabilitata) della chat</t>
+    <t>LobbyStatusAndSettings</t>
+  </si>
+  <si>
+    <t>Contiene lo stato e le impostazioni della partita nella lobby</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Gestita disconnessione di uno dei client (solo lobby)
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220B0B0C-71A4-46C8-9779-DFB99D2073B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EF081-30BA-49F1-B730-5FA67782189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nome Messaggio</t>
   </si>
@@ -36,21 +36,6 @@
     <t>Descrizione</t>
   </si>
   <si>
-    <t>Tipo*</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>0=&gt;MultiDirezione</t>
-  </si>
-  <si>
-    <t>1=&gt;Host verso client</t>
-  </si>
-  <si>
-    <t>2=&gt;Client verso Host</t>
-  </si>
-  <si>
     <t>SendDataConfirmation</t>
   </si>
   <si>
@@ -85,6 +70,18 @@
   </si>
   <si>
     <t>Contiene lo stato e le impostazioni della partita nella lobby</t>
+  </si>
+  <si>
+    <t>HostDisconnectedMessage</t>
+  </si>
+  <si>
+    <t>Notifica i client che l'host si è disconnesso</t>
+  </si>
+  <si>
+    <t>ClientDisconnectedMessage</t>
+  </si>
+  <si>
+    <t>Notifica l'host che il client si è disconnesso manualmente</t>
   </si>
 </sst>
 </file>
@@ -420,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,7 +432,7 @@
     <col min="6" max="6" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,98 +442,93 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2">
         <v>1000</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1005</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1010</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1015</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1001</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B6">
+        <v>1020</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>1002</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B7">
+        <v>1025</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>1003</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B8">
+        <v>1026</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>1004</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9">
+        <v>1027</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="B7">
-        <v>1005</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Init gestione connessione persa con il client
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EF081-30BA-49F1-B730-5FA67782189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A61F35-E44B-4703-ABAC-07778FB325F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Nome Messaggio</t>
   </si>
@@ -81,7 +81,19 @@
     <t>ClientDisconnectedMessage</t>
   </si>
   <si>
-    <t>Notifica l'host che il client si è disconnesso manualmente</t>
+    <t>Watchdog</t>
+  </si>
+  <si>
+    <t>Watchdog mandato dai client all'host</t>
+  </si>
+  <si>
+    <t>Notifica che un client è stato disconnesso</t>
+  </si>
+  <si>
+    <t>ClientConnectionLost</t>
+  </si>
+  <si>
+    <t>Notifica i client che è stata persa la connessione con uno dei client</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,90 +457,112 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1010</v>
+        <v>1005</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1015</v>
+        <v>1010</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>1020</v>
+        <v>1015</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>1025</v>
+        <v>1020</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>1026</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>1027</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>1028</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Invio ai client dello StartGame e del nome della view
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A61F35-E44B-4703-ABAC-07778FB325F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0FAB53-89D4-45AD-82F0-36F3F9C45F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nome Messaggio</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Notifica i client che è stata persa la connessione con uno dei client</t>
+  </si>
+  <si>
+    <t>StartGameCommandMessage</t>
+  </si>
+  <si>
+    <t>Notifica i client che è stata avviata una partita</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,6 +571,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>1030</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" s="2"/>
     </row>

</xml_diff>

<commit_message>
Invio delle impostazioni della partita con StartGameCommandMessage
</commit_message>
<xml_diff>
--- a/LIB_Communication/MessagesDefinition.xlsx
+++ b/LIB_Communication/MessagesDefinition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renny\Documents\GitHub\ArcadeGamesWpf\LIB_Communication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0FAB53-89D4-45AD-82F0-36F3F9C45F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9BB73E-F1E8-4AEE-96F9-72B2BE81A001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
     <t>StartGameCommandMessage</t>
   </si>
   <si>
-    <t>Notifica i client che è stata avviata una partita</t>
+    <t>Notifica i client che è stata avviata una partita e manda le impostazioni della partita</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>